<commit_message>
Update .xlsx output & .gitignore
</commit_message>
<xml_diff>
--- a/schedule_template.xlsx
+++ b/schedule_template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matheuswestphalen/Projects/ScheduleMaker/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194F0262-17A8-E14A-9D28-5E61200C2C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CAEE96-86D4-F648-8B25-EA98C72268DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="53560" yWindow="2300" windowWidth="42000" windowHeight="21900" xr2:uid="{9C83FFFC-4C26-404B-AD94-EDBEE256AE25}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -160,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -172,15 +172,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -579,7 +570,7 @@
   <dimension ref="A5:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="125" zoomScaleNormal="136" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,7 +629,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -658,27 +649,27 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>0</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -698,22 +689,22 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>0</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>